<commit_message>
Mise à jour formats HAD Janvier 2023
</commit_message>
<xml_diff>
--- a/formats/excel/HAD/2023/Formats RPSS ANO 23.xlsx
+++ b/formats/excel/HAD/2023/Formats RPSS ANO 23.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/Developpements/Github/formats_pmeasyr/formats/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1 - DOSSIERS NOMINATIFS\AGEORGES\XXX - DIVERS\formats had\Formats janvier 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD956563-B15E-2A4B-8F8D-3D357DBA21BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{124A726A-6902-4578-922A-190F77E90ED6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -30,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="258">
   <si>
     <t>nom</t>
   </si>
@@ -789,13 +787,28 @@
   </si>
   <si>
     <t>Empreinte numérique</t>
+  </si>
+  <si>
+    <t>CRINS</t>
+  </si>
+  <si>
+    <t>CR51</t>
+  </si>
+  <si>
+    <t>Code retour "article 51"</t>
+  </si>
+  <si>
+    <t>Code retour "identifiant national de santé"</t>
+  </si>
+  <si>
+    <t>ART51</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -806,7 +819,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -829,11 +842,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1216,24 +1230,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
-      <selection pane="bottomRight" sqref="A1:G123"/>
+      <selection pane="bottomRight" activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="52.83203125" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="1025" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="52.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="69.7109375" customWidth="1"/>
+    <col min="5" max="1025" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1256,12 +1271,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>132</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B65" si="0">E2+F2-F3</f>
+        <f t="shared" ref="B2:B66" si="0">E2+F2-F3</f>
         <v>0</v>
       </c>
       <c r="C2" t="s">
@@ -1280,7 +1295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>134</v>
       </c>
@@ -1304,7 +1319,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -1328,7 +1343,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1352,7 +1367,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1376,7 +1391,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1400,7 +1415,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1424,7 +1439,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1448,7 +1463,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -1472,7 +1487,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1496,7 +1511,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1520,7 +1535,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1544,7 +1559,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1568,7 +1583,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1592,7 +1607,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1616,7 +1631,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1640,7 +1655,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>150</v>
       </c>
@@ -1664,7 +1679,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1688,7 +1703,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>153</v>
       </c>
@@ -1712,7 +1727,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1736,7 +1751,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1760,7 +1775,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1784,7 +1799,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1808,7 +1823,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>159</v>
       </c>
@@ -1832,7 +1847,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1856,7 +1871,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>162</v>
       </c>
@@ -1880,7 +1895,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="18" customHeight="1">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1904,7 +1919,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1928,7 +1943,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>166</v>
       </c>
@@ -1952,7 +1967,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>168</v>
       </c>
@@ -1976,7 +1991,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>170</v>
       </c>
@@ -2000,7 +2015,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>172</v>
       </c>
@@ -2024,7 +2039,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>174</v>
       </c>
@@ -2048,7 +2063,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2072,7 +2087,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2096,7 +2111,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2120,7 +2135,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2144,7 +2159,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2168,7 +2183,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2192,7 +2207,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2216,7 +2231,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2240,7 +2255,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2264,7 +2279,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>185</v>
       </c>
@@ -2288,7 +2303,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>187</v>
       </c>
@@ -2312,7 +2327,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>189</v>
       </c>
@@ -2336,7 +2351,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>191</v>
       </c>
@@ -2360,7 +2375,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>193</v>
       </c>
@@ -2384,7 +2399,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>195</v>
       </c>
@@ -2408,7 +2423,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>197</v>
       </c>
@@ -2432,7 +2447,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>199</v>
       </c>
@@ -2456,7 +2471,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>13</v>
       </c>
@@ -2480,7 +2495,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>202</v>
       </c>
@@ -2504,7 +2519,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -2528,7 +2543,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>44</v>
       </c>
@@ -2552,7 +2567,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>45</v>
       </c>
@@ -2576,7 +2591,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>46</v>
       </c>
@@ -2600,7 +2615,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>47</v>
       </c>
@@ -2624,7 +2639,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -2648,7 +2663,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -2672,7 +2687,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>50</v>
       </c>
@@ -2696,7 +2711,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>51</v>
       </c>
@@ -2720,7 +2735,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>52</v>
       </c>
@@ -2744,7 +2759,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -2768,7 +2783,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>54</v>
       </c>
@@ -2792,12 +2807,12 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>55</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B123" si="1">E66+F66-F67</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C66" t="s">
@@ -2813,312 +2828,321 @@
         <v>140</v>
       </c>
       <c r="G66" s="1">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>56</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="B67">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C67" t="s">
-        <v>8</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>57</v>
+        <f t="shared" ref="B67:B126" si="1">E67+F67-F68</f>
+        <v>0</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>256</v>
       </c>
       <c r="E67" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" s="1">
         <v>141</v>
       </c>
       <c r="G67" s="1">
-        <f t="shared" ref="G67:G123" si="2">F67+E67-1</f>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1">
         <v>142</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="G68" s="1">
+        <f>F68+E68-1</f>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>56</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E69" s="1">
+        <v>2</v>
+      </c>
+      <c r="F69" s="1">
+        <f>G68+1</f>
+        <v>143</v>
+      </c>
+      <c r="G69" s="1">
+        <f>F69+E69-1</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
         <v>58</v>
       </c>
-      <c r="B68">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C68" t="s">
-        <v>8</v>
-      </c>
-      <c r="D68" s="1" t="s">
+      <c r="B70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E70" s="1">
         <v>2</v>
       </c>
-      <c r="F68" s="1">
-        <v>143</v>
-      </c>
-      <c r="G68" s="1">
-        <f t="shared" si="2"/>
-        <v>144</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="F70" s="1">
+        <f t="shared" ref="F70:F126" si="2">G69+1</f>
+        <v>145</v>
+      </c>
+      <c r="G70" s="1">
+        <f t="shared" ref="G70:G126" si="3">F70+E70-1</f>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
         <v>60</v>
       </c>
-      <c r="B69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C69" t="s">
-        <v>8</v>
-      </c>
-      <c r="D69" s="1" t="s">
+      <c r="B71">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E69" s="1">
-        <v>1</v>
-      </c>
-      <c r="F69" s="1">
-        <v>145</v>
-      </c>
-      <c r="G69" s="1">
-        <f t="shared" si="2"/>
-        <v>145</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="E71" s="1">
+        <v>1</v>
+      </c>
+      <c r="F71" s="1">
+        <f t="shared" si="2"/>
+        <v>147</v>
+      </c>
+      <c r="G71" s="1">
+        <f t="shared" si="3"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
         <v>61</v>
       </c>
-      <c r="B70">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C70" t="s">
-        <v>8</v>
-      </c>
-      <c r="D70" s="1" t="s">
+      <c r="B72">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E70" s="1">
-        <v>1</v>
-      </c>
-      <c r="F70" s="1">
-        <v>146</v>
-      </c>
-      <c r="G70" s="1">
-        <f t="shared" si="2"/>
-        <v>146</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="E72" s="1">
+        <v>1</v>
+      </c>
+      <c r="F72" s="1">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+      <c r="G72" s="1">
+        <f t="shared" si="3"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
         <v>62</v>
       </c>
-      <c r="B71">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C71" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="1" t="s">
+      <c r="B73">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E73" s="1">
         <v>2</v>
       </c>
-      <c r="F71" s="1">
-        <v>147</v>
-      </c>
-      <c r="G71" s="1">
-        <f t="shared" si="2"/>
-        <v>148</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="F73" s="1">
+        <f t="shared" si="2"/>
+        <v>149</v>
+      </c>
+      <c r="G73" s="1">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
         <v>64</v>
       </c>
-      <c r="B72">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C72" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="1" t="s">
+      <c r="B74">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E74" s="1">
         <v>2</v>
       </c>
-      <c r="F72" s="1">
-        <v>149</v>
-      </c>
-      <c r="G72" s="1">
-        <f t="shared" si="2"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="F74" s="1">
+        <f t="shared" si="2"/>
+        <v>151</v>
+      </c>
+      <c r="G74" s="1">
+        <f t="shared" si="3"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
         <v>66</v>
       </c>
-      <c r="B73">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C73" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="1" t="s">
+      <c r="B75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E73" s="1">
-        <v>1</v>
-      </c>
-      <c r="F73" s="1">
-        <v>151</v>
-      </c>
-      <c r="G73" s="1">
-        <f t="shared" si="2"/>
-        <v>151</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="E75" s="1">
+        <v>1</v>
+      </c>
+      <c r="F75" s="1">
+        <f t="shared" si="2"/>
+        <v>153</v>
+      </c>
+      <c r="G75" s="1">
+        <f t="shared" si="3"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
         <v>220</v>
       </c>
-      <c r="B74">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C74" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74" s="1" t="s">
+      <c r="B76">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E74" s="1">
-        <v>1</v>
-      </c>
-      <c r="F74" s="1">
-        <v>152</v>
-      </c>
-      <c r="G74" s="1">
-        <f t="shared" si="2"/>
-        <v>152</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="E76" s="1">
+        <v>1</v>
+      </c>
+      <c r="F76" s="1">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="G76" s="1">
+        <f t="shared" si="3"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
         <v>68</v>
       </c>
-      <c r="B75">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C75" t="s">
-        <v>8</v>
-      </c>
-      <c r="D75" s="1" t="s">
+      <c r="B77">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C77" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E75" s="1">
-        <v>1</v>
-      </c>
-      <c r="F75" s="1">
-        <v>153</v>
-      </c>
-      <c r="G75" s="1">
-        <f t="shared" si="2"/>
-        <v>153</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="E77" s="1">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1">
+        <f t="shared" si="2"/>
+        <v>155</v>
+      </c>
+      <c r="G77" s="1">
+        <f t="shared" si="3"/>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
         <v>70</v>
       </c>
-      <c r="B76">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="B78">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C78" t="s">
         <v>18</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E76" s="1">
+      <c r="E78" s="1">
         <v>4</v>
       </c>
-      <c r="F76" s="1">
-        <v>154</v>
-      </c>
-      <c r="G76" s="1">
-        <f t="shared" si="2"/>
-        <v>157</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="F78" s="1">
+        <f t="shared" si="2"/>
+        <v>156</v>
+      </c>
+      <c r="G78" s="1">
+        <f t="shared" si="3"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
         <v>72</v>
-      </c>
-      <c r="B77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C77" t="s">
-        <v>73</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E77" s="1">
-        <v>10</v>
-      </c>
-      <c r="F77" s="1">
-        <v>158</v>
-      </c>
-      <c r="G77" s="1">
-        <f t="shared" si="2"/>
-        <v>167</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>75</v>
-      </c>
-      <c r="B78">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C78" t="s">
-        <v>73</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E78" s="1">
-        <v>10</v>
-      </c>
-      <c r="F78" s="1">
-        <v>168</v>
-      </c>
-      <c r="G78" s="1">
-        <f t="shared" si="2"/>
-        <v>177</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>76</v>
       </c>
       <c r="B79">
         <f t="shared" si="1"/>
@@ -3128,22 +3152,23 @@
         <v>73</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>222</v>
+        <v>74</v>
       </c>
       <c r="E79" s="1">
         <v>10</v>
       </c>
       <c r="F79" s="1">
-        <v>178</v>
+        <f t="shared" si="2"/>
+        <v>160</v>
       </c>
       <c r="G79" s="1">
-        <f t="shared" si="2"/>
-        <v>187</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>223</v>
+        <v>75</v>
       </c>
       <c r="B80">
         <f t="shared" si="1"/>
@@ -3153,22 +3178,23 @@
         <v>73</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>77</v>
+        <v>221</v>
       </c>
       <c r="E80" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F80" s="1">
-        <v>188</v>
+        <f t="shared" si="2"/>
+        <v>170</v>
       </c>
       <c r="G80" s="1">
-        <f t="shared" si="2"/>
-        <v>191</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B81">
         <f t="shared" si="1"/>
@@ -3178,22 +3204,23 @@
         <v>73</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>79</v>
+        <v>222</v>
       </c>
       <c r="E81" s="1">
         <v>10</v>
       </c>
       <c r="F81" s="1">
-        <v>192</v>
+        <f t="shared" si="2"/>
+        <v>180</v>
       </c>
       <c r="G81" s="1">
-        <f t="shared" si="2"/>
-        <v>201</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>223</v>
       </c>
       <c r="B82">
         <f t="shared" si="1"/>
@@ -3203,1078 +3230,1166 @@
         <v>73</v>
       </c>
       <c r="D82" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E82" s="1">
+        <v>4</v>
+      </c>
+      <c r="F82" s="1">
+        <f t="shared" si="2"/>
+        <v>190</v>
+      </c>
+      <c r="G82" s="1">
+        <f t="shared" si="3"/>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
+        <v>78</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C83" t="s">
+        <v>73</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E83" s="1">
+        <v>10</v>
+      </c>
+      <c r="F83" s="1">
+        <f t="shared" si="2"/>
+        <v>194</v>
+      </c>
+      <c r="G83" s="1">
+        <f t="shared" si="3"/>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>80</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C84" t="s">
+        <v>73</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E82" s="1">
+      <c r="E84" s="1">
         <v>5</v>
       </c>
-      <c r="F82" s="1">
-        <v>202</v>
-      </c>
-      <c r="G82" s="1">
-        <f t="shared" si="2"/>
-        <v>206</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="F84" s="1">
+        <f t="shared" si="2"/>
+        <v>204</v>
+      </c>
+      <c r="G84" s="1">
+        <f t="shared" si="3"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
         <v>82</v>
       </c>
-      <c r="B83">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C83" t="s">
-        <v>8</v>
-      </c>
-      <c r="D83" s="1" t="s">
+      <c r="B85">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C85" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E83" s="1">
-        <v>1</v>
-      </c>
-      <c r="F83" s="1">
-        <v>207</v>
-      </c>
-      <c r="G83" s="1">
-        <f t="shared" si="2"/>
-        <v>207</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="E85" s="1">
+        <v>1</v>
+      </c>
+      <c r="F85" s="1">
+        <f t="shared" si="2"/>
+        <v>209</v>
+      </c>
+      <c r="G85" s="1">
+        <f t="shared" si="3"/>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
         <v>224</v>
       </c>
-      <c r="B84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C84" t="s">
-        <v>8</v>
-      </c>
-      <c r="D84" s="1" t="s">
+      <c r="B86">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="E84" s="1">
+      <c r="E86" s="1">
         <v>20</v>
       </c>
-      <c r="F84" s="1">
-        <v>208</v>
-      </c>
-      <c r="G84" s="1">
-        <f t="shared" si="2"/>
+      <c r="F86" s="1">
+        <f t="shared" si="2"/>
+        <v>210</v>
+      </c>
+      <c r="G86" s="1">
+        <f t="shared" si="3"/>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>226</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C87" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>226</v>
-      </c>
-      <c r="B85">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C85" t="s">
-        <v>8</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E85" s="1">
-        <v>1</v>
-      </c>
-      <c r="F85" s="1">
+      <c r="E87" s="1">
+        <v>1</v>
+      </c>
+      <c r="F87" s="1">
+        <f t="shared" si="2"/>
+        <v>230</v>
+      </c>
+      <c r="G87" s="1">
+        <f t="shared" si="3"/>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
         <v>228</v>
       </c>
-      <c r="G85" s="1">
-        <f t="shared" si="2"/>
-        <v>228</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>228</v>
-      </c>
-      <c r="B86">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C86" t="s">
-        <v>8</v>
-      </c>
-      <c r="D86" s="1" t="s">
+      <c r="B88">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C88" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E86" s="1">
-        <v>1</v>
-      </c>
-      <c r="F86" s="1">
-        <v>229</v>
-      </c>
-      <c r="G86" s="1">
-        <f t="shared" si="2"/>
-        <v>229</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="E88" s="1">
+        <v>1</v>
+      </c>
+      <c r="F88" s="1">
+        <f t="shared" si="2"/>
+        <v>231</v>
+      </c>
+      <c r="G88" s="1">
+        <f t="shared" si="3"/>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
         <v>84</v>
       </c>
-      <c r="B87">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C87" t="s">
-        <v>8</v>
-      </c>
-      <c r="D87" s="1" t="s">
+      <c r="B89">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C89" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E87" s="1">
-        <v>8</v>
-      </c>
-      <c r="F87" s="1">
-        <v>230</v>
-      </c>
-      <c r="G87" s="1">
-        <f t="shared" si="2"/>
+      <c r="E89" s="1">
+        <v>8</v>
+      </c>
+      <c r="F89" s="1">
+        <f t="shared" si="2"/>
+        <v>232</v>
+      </c>
+      <c r="G89" s="1">
+        <f t="shared" si="3"/>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>231</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C90" t="s">
+        <v>73</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E90" s="1">
+        <v>10</v>
+      </c>
+      <c r="F90" s="1">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+      <c r="G90" s="1">
+        <f t="shared" si="3"/>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" t="s">
+        <v>232</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C91" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E91" s="1">
+        <v>8</v>
+      </c>
+      <c r="F91" s="1">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="G91" s="1">
+        <f t="shared" si="3"/>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>234</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C92" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E92" s="1">
+        <v>1</v>
+      </c>
+      <c r="F92" s="1">
+        <f t="shared" si="2"/>
+        <v>258</v>
+      </c>
+      <c r="G92" s="1">
+        <f t="shared" si="3"/>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E93" s="1">
+        <v>1</v>
+      </c>
+      <c r="F93" s="1">
+        <f t="shared" si="2"/>
+        <v>259</v>
+      </c>
+      <c r="G93" s="1">
+        <f t="shared" si="3"/>
+        <v>259</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>231</v>
-      </c>
-      <c r="B88">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C88" t="s">
+      <c r="B94">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C94" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E94" s="1">
+        <v>9</v>
+      </c>
+      <c r="F94" s="1">
+        <f t="shared" si="2"/>
+        <v>260</v>
+      </c>
+      <c r="G94" s="1">
+        <f t="shared" si="3"/>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
+        <v>87</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C95" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1</v>
+      </c>
+      <c r="F95" s="1">
+        <f t="shared" si="2"/>
+        <v>269</v>
+      </c>
+      <c r="G95" s="1">
+        <f t="shared" si="3"/>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>88</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C96" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E96" s="1">
+        <v>3</v>
+      </c>
+      <c r="F96" s="1">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="G96" s="1">
+        <f t="shared" si="3"/>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
+        <v>89</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C97" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E97" s="1">
+        <v>3</v>
+      </c>
+      <c r="F97" s="1">
+        <f t="shared" si="2"/>
+        <v>273</v>
+      </c>
+      <c r="G97" s="1">
+        <f t="shared" si="3"/>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" t="s">
+        <v>91</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C98" t="s">
+        <v>8</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E98" s="1">
+        <v>4</v>
+      </c>
+      <c r="F98" s="1">
+        <f t="shared" si="2"/>
+        <v>276</v>
+      </c>
+      <c r="G98" s="1">
+        <f t="shared" si="3"/>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
+        <v>92</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C99" t="s">
+        <v>8</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E99" s="1">
+        <v>1</v>
+      </c>
+      <c r="F99" s="1">
+        <f t="shared" si="2"/>
+        <v>280</v>
+      </c>
+      <c r="G99" s="1">
+        <f t="shared" si="3"/>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
+        <v>94</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C100" t="s">
+        <v>8</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E100" s="1">
+        <v>9</v>
+      </c>
+      <c r="F100" s="1">
+        <f t="shared" si="2"/>
+        <v>281</v>
+      </c>
+      <c r="G100" s="1">
+        <f t="shared" si="3"/>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" t="s">
+        <v>95</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C101" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E101" s="1">
+        <v>10</v>
+      </c>
+      <c r="F101" s="1">
+        <f t="shared" si="2"/>
+        <v>290</v>
+      </c>
+      <c r="G101" s="1">
+        <f t="shared" si="3"/>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" t="s">
+        <v>96</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C102" t="s">
+        <v>8</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E102" s="1">
+        <v>1</v>
+      </c>
+      <c r="F102" s="1">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="G102" s="1">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" t="s">
+        <v>244</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C103" t="s">
+        <v>8</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E103" s="1">
+        <v>8</v>
+      </c>
+      <c r="F103" s="1">
+        <f t="shared" si="2"/>
+        <v>301</v>
+      </c>
+      <c r="G103" s="1">
+        <f t="shared" si="3"/>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" t="s">
+        <v>245</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C104" t="s">
+        <v>8</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E104" s="1">
+        <v>8</v>
+      </c>
+      <c r="F104" s="1">
+        <f t="shared" si="2"/>
+        <v>309</v>
+      </c>
+      <c r="G104" s="1">
+        <f t="shared" si="3"/>
+        <v>316</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" t="s">
+        <v>246</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C105" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E105" s="1">
+        <v>3</v>
+      </c>
+      <c r="F105" s="1">
+        <f t="shared" si="2"/>
+        <v>317</v>
+      </c>
+      <c r="G105" s="1">
+        <f t="shared" si="3"/>
+        <v>319</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" t="s">
+        <v>101</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C106" t="s">
+        <v>8</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E106" s="1">
+        <v>3</v>
+      </c>
+      <c r="F106" s="1">
+        <f t="shared" si="2"/>
+        <v>320</v>
+      </c>
+      <c r="G106" s="1">
+        <f t="shared" si="3"/>
+        <v>322</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" t="s">
+        <v>247</v>
+      </c>
+      <c r="B107">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C107" t="s">
+        <v>8</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E107" s="1">
+        <v>1</v>
+      </c>
+      <c r="F107" s="1">
+        <f t="shared" si="2"/>
+        <v>323</v>
+      </c>
+      <c r="G107" s="1">
+        <f t="shared" si="3"/>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" t="s">
+        <v>19</v>
+      </c>
+      <c r="B108">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C108" t="s">
+        <v>8</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E108" s="1">
+        <v>8</v>
+      </c>
+      <c r="F108" s="1">
+        <f t="shared" si="2"/>
+        <v>324</v>
+      </c>
+      <c r="G108" s="1">
+        <f t="shared" si="3"/>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" t="s">
+        <v>248</v>
+      </c>
+      <c r="B109">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C109" t="s">
+        <v>8</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E109" s="1">
+        <v>8</v>
+      </c>
+      <c r="F109" s="1">
+        <f t="shared" si="2"/>
+        <v>332</v>
+      </c>
+      <c r="G109" s="1">
+        <f t="shared" si="3"/>
+        <v>339</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" t="s">
+        <v>106</v>
+      </c>
+      <c r="B110">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C110" t="s">
         <v>73</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E88" s="1">
-        <v>10</v>
-      </c>
-      <c r="F88" s="1">
-        <v>238</v>
-      </c>
-      <c r="G88" s="1">
-        <f t="shared" si="2"/>
-        <v>247</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>232</v>
-      </c>
-      <c r="B89">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C89" t="s">
-        <v>8</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E89" s="1">
-        <v>8</v>
-      </c>
-      <c r="F89" s="1">
-        <v>248</v>
-      </c>
-      <c r="G89" s="1">
-        <f t="shared" si="2"/>
-        <v>255</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>234</v>
-      </c>
-      <c r="B90">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C90" t="s">
-        <v>8</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E90" s="1">
-        <v>1</v>
-      </c>
-      <c r="F90" s="1">
-        <v>256</v>
-      </c>
-      <c r="G90" s="1">
-        <f t="shared" si="2"/>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>86</v>
-      </c>
-      <c r="B91">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C91" t="s">
-        <v>8</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="E91" s="1">
-        <v>1</v>
-      </c>
-      <c r="F91" s="1">
+      <c r="D110" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E110" s="1">
+        <v>8</v>
+      </c>
+      <c r="F110" s="1">
+        <f t="shared" si="2"/>
+        <v>340</v>
+      </c>
+      <c r="G110" s="1">
+        <f t="shared" si="3"/>
+        <v>347</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" t="s">
+        <v>108</v>
+      </c>
+      <c r="B111">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C111" t="s">
+        <v>8</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E111" s="1">
+        <v>1</v>
+      </c>
+      <c r="F111" s="1">
+        <f t="shared" si="2"/>
+        <v>348</v>
+      </c>
+      <c r="G111" s="1">
+        <f t="shared" si="3"/>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" t="s">
+        <v>110</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C112" t="s">
+        <v>8</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E112" s="1">
+        <v>8</v>
+      </c>
+      <c r="F112" s="1">
+        <f t="shared" si="2"/>
+        <v>349</v>
+      </c>
+      <c r="G112" s="1">
+        <f t="shared" si="3"/>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C113" t="s">
+        <v>8</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E113" s="1">
+        <v>8</v>
+      </c>
+      <c r="F113" s="1">
+        <f t="shared" si="2"/>
+        <v>357</v>
+      </c>
+      <c r="G113" s="1">
+        <f t="shared" si="3"/>
+        <v>364</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" t="s">
+        <v>114</v>
+      </c>
+      <c r="B114">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C114" t="s">
+        <v>8</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E114" s="1">
+        <v>8</v>
+      </c>
+      <c r="F114" s="1">
+        <f t="shared" si="2"/>
+        <v>365</v>
+      </c>
+      <c r="G114" s="1">
+        <f t="shared" si="3"/>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" t="s">
+        <v>116</v>
+      </c>
+      <c r="B115">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C115" t="s">
+        <v>8</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E115" s="1">
+        <v>8</v>
+      </c>
+      <c r="F115" s="1">
+        <f t="shared" si="2"/>
+        <v>373</v>
+      </c>
+      <c r="G115" s="1">
+        <f t="shared" si="3"/>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" t="s">
+        <v>118</v>
+      </c>
+      <c r="B116">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C116" t="s">
+        <v>8</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E116" s="1">
+        <v>8</v>
+      </c>
+      <c r="F116" s="1">
+        <f t="shared" si="2"/>
+        <v>381</v>
+      </c>
+      <c r="G116" s="1">
+        <f t="shared" si="3"/>
+        <v>388</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117" t="s">
+        <v>120</v>
+      </c>
+      <c r="B117">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C117" t="s">
+        <v>8</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E117" s="1">
+        <v>8</v>
+      </c>
+      <c r="F117" s="1">
+        <f t="shared" si="2"/>
+        <v>389</v>
+      </c>
+      <c r="G117" s="1">
+        <f t="shared" si="3"/>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" t="s">
+        <v>122</v>
+      </c>
+      <c r="B118">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C118" t="s">
+        <v>8</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E118" s="1">
+        <v>1</v>
+      </c>
+      <c r="F118" s="1">
+        <f t="shared" si="2"/>
+        <v>397</v>
+      </c>
+      <c r="G118" s="1">
+        <f t="shared" si="3"/>
+        <v>397</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" t="s">
+        <v>124</v>
+      </c>
+      <c r="B119">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C119" t="s">
+        <v>8</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E119" s="1">
+        <v>1</v>
+      </c>
+      <c r="F119" s="1">
+        <f t="shared" si="2"/>
+        <v>398</v>
+      </c>
+      <c r="G119" s="1">
+        <f t="shared" si="3"/>
+        <v>398</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" t="s">
+        <v>126</v>
+      </c>
+      <c r="B120">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C120" t="s">
+        <v>8</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E120" s="1">
+        <v>1</v>
+      </c>
+      <c r="F120" s="1">
+        <f t="shared" si="2"/>
+        <v>399</v>
+      </c>
+      <c r="G120" s="1">
+        <f t="shared" si="3"/>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" t="s">
+        <v>128</v>
+      </c>
+      <c r="B121">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C121" t="s">
+        <v>8</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E121" s="1">
+        <v>3</v>
+      </c>
+      <c r="F121" s="1">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+      <c r="G121" s="1">
+        <f t="shared" si="3"/>
+        <v>402</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" t="s">
+        <v>249</v>
+      </c>
+      <c r="B122">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C122" t="s">
+        <v>8</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E122" s="1">
+        <v>20</v>
+      </c>
+      <c r="F122" s="1">
+        <f t="shared" si="2"/>
+        <v>403</v>
+      </c>
+      <c r="G122" s="1">
+        <f t="shared" si="3"/>
+        <v>422</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" t="s">
         <v>257</v>
       </c>
-      <c r="G91" s="1">
-        <f t="shared" si="2"/>
+      <c r="B123">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C123" t="s">
+        <v>8</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>237</v>
-      </c>
-      <c r="B92">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C92" t="s">
-        <v>8</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E92" s="1">
-        <v>9</v>
-      </c>
-      <c r="F92" s="1">
-        <v>258</v>
-      </c>
-      <c r="G92" s="1">
-        <f t="shared" si="2"/>
-        <v>266</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>87</v>
-      </c>
-      <c r="B93">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C93" t="s">
-        <v>8</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E93" s="1">
-        <v>1</v>
-      </c>
-      <c r="F93" s="1">
-        <v>267</v>
-      </c>
-      <c r="G93" s="1">
-        <f t="shared" si="2"/>
-        <v>267</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>88</v>
-      </c>
-      <c r="B94">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C94" t="s">
-        <v>8</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E94" s="1">
-        <v>3</v>
-      </c>
-      <c r="F94" s="1">
-        <v>268</v>
-      </c>
-      <c r="G94" s="1">
-        <f t="shared" si="2"/>
-        <v>270</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>89</v>
-      </c>
-      <c r="B95">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C95" t="s">
-        <v>8</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E95" s="1">
-        <v>3</v>
-      </c>
-      <c r="F95" s="1">
-        <v>271</v>
-      </c>
-      <c r="G95" s="1">
-        <f t="shared" si="2"/>
-        <v>273</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>91</v>
-      </c>
-      <c r="B96">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C96" t="s">
-        <v>8</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E96" s="1">
-        <v>4</v>
-      </c>
-      <c r="F96" s="1">
-        <v>274</v>
-      </c>
-      <c r="G96" s="1">
-        <f t="shared" si="2"/>
-        <v>277</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>92</v>
-      </c>
-      <c r="B97">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C97" t="s">
-        <v>8</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E97" s="1">
-        <v>1</v>
-      </c>
-      <c r="F97" s="1">
-        <v>278</v>
-      </c>
-      <c r="G97" s="1">
-        <f t="shared" si="2"/>
-        <v>278</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>94</v>
-      </c>
-      <c r="B98">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C98" t="s">
-        <v>8</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E98" s="1">
-        <v>9</v>
-      </c>
-      <c r="F98" s="1">
-        <v>279</v>
-      </c>
-      <c r="G98" s="1">
-        <f t="shared" si="2"/>
-        <v>287</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>95</v>
-      </c>
-      <c r="B99">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C99" t="s">
-        <v>8</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E99" s="1">
-        <v>10</v>
-      </c>
-      <c r="F99" s="1">
-        <v>288</v>
-      </c>
-      <c r="G99" s="1">
-        <f t="shared" si="2"/>
-        <v>297</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>96</v>
-      </c>
-      <c r="B100">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C100" t="s">
-        <v>8</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E100" s="1">
-        <v>1</v>
-      </c>
-      <c r="F100" s="1">
-        <v>298</v>
-      </c>
-      <c r="G100" s="1">
-        <f t="shared" si="2"/>
-        <v>298</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>244</v>
-      </c>
-      <c r="B101">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C101" t="s">
-        <v>8</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E101" s="1">
-        <v>8</v>
-      </c>
-      <c r="F101" s="1">
-        <v>299</v>
-      </c>
-      <c r="G101" s="1">
-        <f t="shared" si="2"/>
-        <v>306</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>245</v>
-      </c>
-      <c r="B102">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C102" t="s">
-        <v>8</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E102" s="1">
-        <v>8</v>
-      </c>
-      <c r="F102" s="1">
-        <v>307</v>
-      </c>
-      <c r="G102" s="1">
-        <f t="shared" si="2"/>
-        <v>314</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>246</v>
-      </c>
-      <c r="B103">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C103" t="s">
-        <v>8</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E103" s="1">
-        <v>3</v>
-      </c>
-      <c r="F103" s="1">
-        <v>315</v>
-      </c>
-      <c r="G103" s="1">
-        <f t="shared" si="2"/>
-        <v>317</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>101</v>
-      </c>
-      <c r="B104">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C104" t="s">
-        <v>8</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E104" s="1">
-        <v>3</v>
-      </c>
-      <c r="F104" s="1">
-        <v>318</v>
-      </c>
-      <c r="G104" s="1">
-        <f t="shared" si="2"/>
-        <v>320</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>247</v>
-      </c>
-      <c r="B105">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C105" t="s">
-        <v>8</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E105" s="1">
-        <v>1</v>
-      </c>
-      <c r="F105" s="1">
-        <v>321</v>
-      </c>
-      <c r="G105" s="1">
-        <f t="shared" si="2"/>
-        <v>321</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>19</v>
-      </c>
-      <c r="B106">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C106" t="s">
-        <v>8</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E106" s="1">
-        <v>8</v>
-      </c>
-      <c r="F106" s="1">
-        <v>322</v>
-      </c>
-      <c r="G106" s="1">
-        <f t="shared" si="2"/>
-        <v>329</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>248</v>
-      </c>
-      <c r="B107">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C107" t="s">
-        <v>8</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E107" s="1">
-        <v>8</v>
-      </c>
-      <c r="F107" s="1">
-        <v>330</v>
-      </c>
-      <c r="G107" s="1">
-        <f t="shared" si="2"/>
-        <v>337</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>106</v>
-      </c>
-      <c r="B108">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C108" t="s">
-        <v>73</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E108" s="1">
-        <v>8</v>
-      </c>
-      <c r="F108" s="1">
-        <v>338</v>
-      </c>
-      <c r="G108" s="1">
-        <f t="shared" si="2"/>
-        <v>345</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>108</v>
-      </c>
-      <c r="B109">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C109" t="s">
-        <v>8</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E109" s="1">
-        <v>1</v>
-      </c>
-      <c r="F109" s="1">
-        <v>346</v>
-      </c>
-      <c r="G109" s="1">
-        <f t="shared" si="2"/>
-        <v>346</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>110</v>
-      </c>
-      <c r="B110">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C110" t="s">
-        <v>8</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E110" s="1">
-        <v>8</v>
-      </c>
-      <c r="F110" s="1">
-        <v>347</v>
-      </c>
-      <c r="G110" s="1">
-        <f t="shared" si="2"/>
-        <v>354</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>112</v>
-      </c>
-      <c r="B111">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C111" t="s">
-        <v>8</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E111" s="1">
-        <v>8</v>
-      </c>
-      <c r="F111" s="1">
-        <v>355</v>
-      </c>
-      <c r="G111" s="1">
-        <f t="shared" si="2"/>
-        <v>362</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
-        <v>114</v>
-      </c>
-      <c r="B112">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C112" t="s">
-        <v>8</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E112" s="1">
-        <v>8</v>
-      </c>
-      <c r="F112" s="1">
-        <v>363</v>
-      </c>
-      <c r="G112" s="1">
-        <f t="shared" si="2"/>
-        <v>370</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>116</v>
-      </c>
-      <c r="B113">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C113" t="s">
-        <v>8</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E113" s="1">
-        <v>8</v>
-      </c>
-      <c r="F113" s="1">
-        <v>371</v>
-      </c>
-      <c r="G113" s="1">
-        <f t="shared" si="2"/>
-        <v>378</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>118</v>
-      </c>
-      <c r="B114">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C114" t="s">
-        <v>8</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E114" s="1">
-        <v>8</v>
-      </c>
-      <c r="F114" s="1">
-        <v>379</v>
-      </c>
-      <c r="G114" s="1">
-        <f t="shared" si="2"/>
-        <v>386</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>120</v>
-      </c>
-      <c r="B115">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C115" t="s">
-        <v>8</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E115" s="1">
-        <v>8</v>
-      </c>
-      <c r="F115" s="1">
-        <v>387</v>
-      </c>
-      <c r="G115" s="1">
-        <f t="shared" si="2"/>
-        <v>394</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>122</v>
-      </c>
-      <c r="B116">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C116" t="s">
-        <v>8</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E116" s="1">
-        <v>1</v>
-      </c>
-      <c r="F116" s="1">
-        <v>395</v>
-      </c>
-      <c r="G116" s="1">
-        <f t="shared" si="2"/>
-        <v>395</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>124</v>
-      </c>
-      <c r="B117">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C117" t="s">
-        <v>8</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E117" s="1">
-        <v>1</v>
-      </c>
-      <c r="F117" s="1">
-        <v>396</v>
-      </c>
-      <c r="G117" s="1">
-        <f t="shared" si="2"/>
-        <v>396</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>126</v>
-      </c>
-      <c r="B118">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C118" t="s">
-        <v>8</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E118" s="1">
-        <v>1</v>
-      </c>
-      <c r="F118" s="1">
-        <v>397</v>
-      </c>
-      <c r="G118" s="1">
-        <f t="shared" si="2"/>
-        <v>397</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>128</v>
-      </c>
-      <c r="B119">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C119" t="s">
-        <v>8</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E119" s="1">
-        <v>3</v>
-      </c>
-      <c r="F119" s="1">
-        <v>398</v>
-      </c>
-      <c r="G119" s="1">
-        <f t="shared" si="2"/>
-        <v>400</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>249</v>
-      </c>
-      <c r="B120">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C120" t="s">
-        <v>8</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E120" s="1">
-        <v>20</v>
-      </c>
-      <c r="F120" s="1">
-        <v>401</v>
-      </c>
-      <c r="G120" s="1">
-        <f t="shared" si="2"/>
-        <v>420</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+      <c r="E123" s="1">
+        <v>1</v>
+      </c>
+      <c r="F123" s="1">
+        <f t="shared" si="2"/>
+        <v>423</v>
+      </c>
+      <c r="G123" s="1">
+        <f t="shared" si="3"/>
+        <v>423</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" t="s">
         <v>33</v>
       </c>
-      <c r="B121">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C121" t="s">
-        <v>8</v>
-      </c>
-      <c r="D121" s="1" t="s">
+      <c r="B124">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C124" t="s">
+        <v>8</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E121" s="1">
+      <c r="E124" s="1">
         <v>50</v>
       </c>
-      <c r="F121" s="1">
-        <v>421</v>
-      </c>
-      <c r="G121" s="1">
-        <f t="shared" si="2"/>
-        <v>470</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
+      <c r="F124" s="1">
+        <f t="shared" si="2"/>
+        <v>424</v>
+      </c>
+      <c r="G124" s="1">
+        <f t="shared" si="3"/>
+        <v>473</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" t="s">
         <v>251</v>
       </c>
-      <c r="B122">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C122" t="s">
-        <v>8</v>
-      </c>
-      <c r="D122" s="1" t="s">
+      <c r="B125">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C125" t="s">
+        <v>8</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E122" s="1">
+      <c r="E125" s="1">
         <v>32</v>
       </c>
-      <c r="F122" s="1">
-        <v>471</v>
-      </c>
-      <c r="G122" s="1">
-        <f t="shared" si="2"/>
-        <v>502</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+      <c r="F125" s="1">
+        <f t="shared" si="2"/>
+        <v>474</v>
+      </c>
+      <c r="G125" s="1">
+        <f t="shared" si="3"/>
+        <v>505</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" t="s">
         <v>130</v>
       </c>
-      <c r="B123">
-        <f t="shared" si="1"/>
-        <v>1284</v>
-      </c>
-      <c r="C123" t="s">
-        <v>8</v>
-      </c>
-      <c r="D123" s="1" t="s">
+      <c r="B126">
+        <f t="shared" si="1"/>
+        <v>1287</v>
+      </c>
+      <c r="C126" t="s">
+        <v>8</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E123" s="1">
+      <c r="E126" s="1">
         <v>781</v>
       </c>
-      <c r="F123" s="1">
-        <v>503</v>
-      </c>
-      <c r="G123" s="1">
-        <f t="shared" si="2"/>
-        <v>1283</v>
+      <c r="F126" s="1">
+        <f t="shared" si="2"/>
+        <v>506</v>
+      </c>
+      <c r="G126" s="1">
+        <f t="shared" si="3"/>
+        <v>1286</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.69930555555555496" right="0.69930555555555496" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1025" width="9" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.69930555555555496" right="0.69930555555555496" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1025" width="9" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.69930555555555496" right="0.69930555555555496" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
 </file>
</xml_diff>